<commit_message>
Additional recording periods added to recording period graph.
</commit_message>
<xml_diff>
--- a/phase1_analysis/data/BD2025_period_subset.xlsx
+++ b/phase1_analysis/data/BD2025_period_subset.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D112"/>
+  <dimension ref="A1:D186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1862,7 +1862,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -1876,13 +1876,13 @@
         </is>
       </c>
       <c r="D76">
-        <v>31</v>
+        <v>71</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -1896,13 +1896,13 @@
         </is>
       </c>
       <c r="D77">
-        <v>35</v>
+        <v>81</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1916,13 +1916,13 @@
         </is>
       </c>
       <c r="D78">
-        <v>26</v>
+        <v>75</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -1936,13 +1936,13 @@
         </is>
       </c>
       <c r="D79">
-        <v>27</v>
+        <v>69</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -1956,13 +1956,13 @@
         </is>
       </c>
       <c r="D80">
-        <v>34</v>
+        <v>75</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -1976,13 +1976,13 @@
         </is>
       </c>
       <c r="D81">
-        <v>39</v>
+        <v>82</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -1996,13 +1996,13 @@
         </is>
       </c>
       <c r="D82">
-        <v>34</v>
+        <v>81</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2016,13 +2016,13 @@
         </is>
       </c>
       <c r="D83">
-        <v>29</v>
+        <v>69</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2036,13 +2036,13 @@
         </is>
       </c>
       <c r="D84">
-        <v>32</v>
+        <v>79</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2056,13 +2056,13 @@
         </is>
       </c>
       <c r="D85">
-        <v>26</v>
+        <v>51</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2076,13 +2076,13 @@
         </is>
       </c>
       <c r="D86">
-        <v>35</v>
+        <v>93</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2096,13 +2096,13 @@
         </is>
       </c>
       <c r="D87">
-        <v>28</v>
+        <v>63</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2116,13 +2116,13 @@
         </is>
       </c>
       <c r="D88">
-        <v>43</v>
+        <v>81</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2136,13 +2136,13 @@
         </is>
       </c>
       <c r="D89">
-        <v>33</v>
+        <v>76</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2156,13 +2156,13 @@
         </is>
       </c>
       <c r="D90">
-        <v>32</v>
+        <v>74</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -2176,13 +2176,13 @@
         </is>
       </c>
       <c r="D91">
-        <v>35</v>
+        <v>77</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -2196,13 +2196,13 @@
         </is>
       </c>
       <c r="D92">
-        <v>28</v>
+        <v>72</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -2216,13 +2216,13 @@
         </is>
       </c>
       <c r="D93">
-        <v>35</v>
+        <v>59</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -2236,13 +2236,13 @@
         </is>
       </c>
       <c r="D94">
-        <v>34</v>
+        <v>75</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -2256,13 +2256,13 @@
         </is>
       </c>
       <c r="D95">
-        <v>35</v>
+        <v>68</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -2276,13 +2276,13 @@
         </is>
       </c>
       <c r="D96">
-        <v>37</v>
+        <v>81</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -2296,13 +2296,13 @@
         </is>
       </c>
       <c r="D97">
-        <v>36</v>
+        <v>61</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -2316,13 +2316,13 @@
         </is>
       </c>
       <c r="D98">
-        <v>38</v>
+        <v>78</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2336,13 +2336,13 @@
         </is>
       </c>
       <c r="D99">
-        <v>49</v>
+        <v>89</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2356,13 +2356,13 @@
         </is>
       </c>
       <c r="D100">
-        <v>38</v>
+        <v>77</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2376,13 +2376,13 @@
         </is>
       </c>
       <c r="D101">
-        <v>35</v>
+        <v>61</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2396,13 +2396,13 @@
         </is>
       </c>
       <c r="D102">
-        <v>51</v>
+        <v>88</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2416,13 +2416,13 @@
         </is>
       </c>
       <c r="D103">
-        <v>33</v>
+        <v>79</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2436,13 +2436,13 @@
         </is>
       </c>
       <c r="D104">
-        <v>37</v>
+        <v>64</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -2456,13 +2456,13 @@
         </is>
       </c>
       <c r="D105">
-        <v>28</v>
+        <v>56</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2476,13 +2476,13 @@
         </is>
       </c>
       <c r="D106">
-        <v>34</v>
+        <v>71</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -2496,13 +2496,13 @@
         </is>
       </c>
       <c r="D107">
-        <v>44</v>
+        <v>73</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -2516,13 +2516,13 @@
         </is>
       </c>
       <c r="D108">
-        <v>49</v>
+        <v>69</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -2536,13 +2536,13 @@
         </is>
       </c>
       <c r="D109">
-        <v>33</v>
+        <v>69</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -2556,13 +2556,13 @@
         </is>
       </c>
       <c r="D110">
-        <v>35</v>
+        <v>59</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>dusk</t>
+          <t>day</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -2576,27 +2576,1507 @@
         </is>
       </c>
       <c r="D111">
-        <v>32</v>
+        <v>58</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Audiomoth_9</t>
+        </is>
+      </c>
+      <c r="D112">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
           <t>dusk</t>
         </is>
       </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>BDWD</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Audiomoth_1</t>
+        </is>
+      </c>
+      <c r="D113">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Audiomoth_10</t>
+        </is>
+      </c>
+      <c r="D114">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Audiomoth_11</t>
+        </is>
+      </c>
+      <c r="D115">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Audiomoth_12</t>
+        </is>
+      </c>
+      <c r="D116">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Audiomoth_13</t>
+        </is>
+      </c>
+      <c r="D117">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Audiomoth_14</t>
+        </is>
+      </c>
+      <c r="D118">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Audiomoth_15</t>
+        </is>
+      </c>
+      <c r="D119">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Audiomoth_16</t>
+        </is>
+      </c>
+      <c r="D120">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Audiomoth_17</t>
+        </is>
+      </c>
+      <c r="D121">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Audiomoth_18</t>
+        </is>
+      </c>
+      <c r="D122">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Audiomoth_2</t>
+        </is>
+      </c>
+      <c r="D123">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Audiomoth_20</t>
+        </is>
+      </c>
+      <c r="D124">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Audiomoth_3</t>
+        </is>
+      </c>
+      <c r="D125">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Audiomoth_4</t>
+        </is>
+      </c>
+      <c r="D126">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Audiomoth_5</t>
+        </is>
+      </c>
+      <c r="D127">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Audiomoth_6</t>
+        </is>
+      </c>
+      <c r="D128">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Audiomoth_7</t>
+        </is>
+      </c>
+      <c r="D129">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Audiomoth_1</t>
+        </is>
+      </c>
+      <c r="D130">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Audiomoth_10</t>
+        </is>
+      </c>
+      <c r="D131">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Audiomoth_11</t>
+        </is>
+      </c>
+      <c r="D132">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Audiomoth_12</t>
+        </is>
+      </c>
+      <c r="D133">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Audiomoth_13</t>
+        </is>
+      </c>
+      <c r="D134">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Audiomoth_14</t>
+        </is>
+      </c>
+      <c r="D135">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Audiomoth_15</t>
+        </is>
+      </c>
+      <c r="D136">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Audiomoth_16</t>
+        </is>
+      </c>
+      <c r="D137">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Audiomoth_17</t>
+        </is>
+      </c>
+      <c r="D138">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Audiomoth_18</t>
+        </is>
+      </c>
+      <c r="D139">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>Audiomoth_19</t>
+        </is>
+      </c>
+      <c r="D140">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Audiomoth_2</t>
+        </is>
+      </c>
+      <c r="D141">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Audiomoth_20</t>
+        </is>
+      </c>
+      <c r="D142">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Audiomoth_3</t>
+        </is>
+      </c>
+      <c r="D143">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Audiomoth_4</t>
+        </is>
+      </c>
+      <c r="D144">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Audiomoth_5</t>
+        </is>
+      </c>
+      <c r="D145">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Audiomoth_6</t>
+        </is>
+      </c>
+      <c r="D146">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Audiomoth_7</t>
+        </is>
+      </c>
+      <c r="D147">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Audiomoth_8</t>
+        </is>
+      </c>
+      <c r="D148">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>dusk</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
         <is>
           <t>Audiomoth_9</t>
         </is>
       </c>
-      <c r="D112">
+      <c r="D149">
         <v>49</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Audiomoth_1</t>
+        </is>
+      </c>
+      <c r="D150">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Audiomoth_10</t>
+        </is>
+      </c>
+      <c r="D151">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>Audiomoth_11</t>
+        </is>
+      </c>
+      <c r="D152">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Audiomoth_12</t>
+        </is>
+      </c>
+      <c r="D153">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>Audiomoth_13</t>
+        </is>
+      </c>
+      <c r="D154">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>Audiomoth_14</t>
+        </is>
+      </c>
+      <c r="D155">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>Audiomoth_15</t>
+        </is>
+      </c>
+      <c r="D156">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>Audiomoth_16</t>
+        </is>
+      </c>
+      <c r="D157">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>Audiomoth_17</t>
+        </is>
+      </c>
+      <c r="D158">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>Audiomoth_18</t>
+        </is>
+      </c>
+      <c r="D159">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>Audiomoth_2</t>
+        </is>
+      </c>
+      <c r="D160">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>Audiomoth_20</t>
+        </is>
+      </c>
+      <c r="D161">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>Audiomoth_3</t>
+        </is>
+      </c>
+      <c r="D162">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>Audiomoth_4</t>
+        </is>
+      </c>
+      <c r="D163">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>Audiomoth_5</t>
+        </is>
+      </c>
+      <c r="D164">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>Audiomoth_6</t>
+        </is>
+      </c>
+      <c r="D165">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>BDMD</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>Audiomoth_7</t>
+        </is>
+      </c>
+      <c r="D166">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>Audiomoth_1</t>
+        </is>
+      </c>
+      <c r="D167">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>Audiomoth_10</t>
+        </is>
+      </c>
+      <c r="D168">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>Audiomoth_11</t>
+        </is>
+      </c>
+      <c r="D169">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>Audiomoth_12</t>
+        </is>
+      </c>
+      <c r="D170">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>Audiomoth_13</t>
+        </is>
+      </c>
+      <c r="D171">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>Audiomoth_14</t>
+        </is>
+      </c>
+      <c r="D172">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>Audiomoth_15</t>
+        </is>
+      </c>
+      <c r="D173">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>Audiomoth_16</t>
+        </is>
+      </c>
+      <c r="D174">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>Audiomoth_17</t>
+        </is>
+      </c>
+      <c r="D175">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>Audiomoth_18</t>
+        </is>
+      </c>
+      <c r="D176">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>Audiomoth_19</t>
+        </is>
+      </c>
+      <c r="D177">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>Audiomoth_2</t>
+        </is>
+      </c>
+      <c r="D178">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>Audiomoth_20</t>
+        </is>
+      </c>
+      <c r="D179">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>Audiomoth_3</t>
+        </is>
+      </c>
+      <c r="D180">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>Audiomoth_4</t>
+        </is>
+      </c>
+      <c r="D181">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>Audiomoth_5</t>
+        </is>
+      </c>
+      <c r="D182">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>Audiomoth_6</t>
+        </is>
+      </c>
+      <c r="D183">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>Audiomoth_7</t>
+        </is>
+      </c>
+      <c r="D184">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>Audiomoth_8</t>
+        </is>
+      </c>
+      <c r="D185">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>night</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>BDWD</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>Audiomoth_9</t>
+        </is>
+      </c>
+      <c r="D186">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>